<commit_message>
Update missing nb-NO strings
</commit_message>
<xml_diff>
--- a/SignalAnalysis/localization/SignalAnalysis string resources.xlsx
+++ b/SignalAnalysis/localization/SignalAnalysis string resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthurit\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C422032-A0A4-484B-8F00-FAA671D9AF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFC0E49-1A3E-4850-AB67-C548A4821E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{8C7C20F6-2391-4792-9F49-F927461B5B85}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3623" uniqueCount="2391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3625" uniqueCount="2393">
   <si>
     <t>File</t>
   </si>
@@ -7442,6 +7431,12 @@
   </si>
   <si>
     <t>Numerisk integrasjon</t>
+  </si>
+  <si>
+    <t>Venstre punktregel, Midtpunktregel, Høyre punktregel, Trapesregel, Simpsons 1/3-regel, Simpsons 3/8-regel, Simpsons sammensatte regel, Rombergs metode</t>
+  </si>
+  <si>
+    <t>Bakover én-punkts differanse, Fremover én-punkts differanse, Sentral tre-punkts differanse, Sentral fem-punkts differanse, Sentral syv-punkts differanse, Sentral ni-punkts differanse, Savitzky–Golay lineær tre-punkts, Savitzky–Golay lineær fem-punkts, Savitzky–Golay lineær syv-punkts, Savitzky–Golay lineær ni-punkts, Savitzky–Golay kubisk fem-punkts, Savitzky–Golay kubisk syv-punkts, Savitzky–Golay kubisk ni-punkts</t>
   </si>
 </sst>
 </file>
@@ -9833,7 +9828,9 @@
       <c r="N34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O34" s="1"/>
+      <c r="O34" s="1" t="s">
+        <v>2392</v>
+      </c>
       <c r="P34" s="1" t="s">
         <v>3</v>
       </c>
@@ -13011,7 +13008,9 @@
       <c r="N88" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O88" s="1"/>
+      <c r="O88" s="1" t="s">
+        <v>2391</v>
+      </c>
       <c r="P88" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>